<commit_message>
added signin and async wait
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik\Downloads\marsframework-master\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428059-39C0-4B90-8BCF-7E49202B9138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4AD7A5-210C-416A-B73B-2E1661EFB367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9492" yWindow="2652" windowWidth="10440" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Url</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mvpstudio.qa@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SydneyQa2018 </t>
   </si>
 </sst>
 </file>
@@ -519,16 +525,16 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -545,7 +551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -574,18 +580,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,15 +602,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -622,23 +628,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="1" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -670,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>

</xml_diff>